<commit_message>
Tweaked LBJ rating curve
</commit_message>
<xml_diff>
--- a/Data/Q/StageCorrection.xlsx
+++ b/Data/Q/StageCorrection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="LBJ" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -126,7 +126,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,184 +701,226 @@
         <v>1445</v>
       </c>
       <c r="C14" s="6">
-        <v>41430</v>
+        <v>41387</v>
       </c>
       <c r="D14" s="1">
-        <v>915</v>
+        <v>1515</v>
       </c>
       <c r="E14" s="5">
         <v>-4.5</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ref="F14:F17" si="1">E14/102</f>
+        <f t="shared" ref="F14:F19" si="1">E14/102</f>
         <v>-4.4117647058823532E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>41430</v>
+        <v>41387</v>
       </c>
       <c r="B15" s="1">
-        <v>930</v>
+        <v>1530</v>
       </c>
       <c r="C15" s="6">
-        <v>41450</v>
+        <v>41405</v>
       </c>
       <c r="D15" s="1">
-        <v>1300</v>
+        <v>1515</v>
       </c>
       <c r="E15" s="5">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>-2.9411764705882353E-2</v>
+        <v>-6.8627450980392163E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="6">
+        <v>41405</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1530</v>
+      </c>
+      <c r="C16" s="6">
+        <v>41430</v>
+      </c>
+      <c r="D16" s="1">
+        <v>915</v>
+      </c>
+      <c r="E16" s="5">
+        <v>-4.5</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>-4.4117647058823532E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>41430</v>
+      </c>
+      <c r="B17" s="1">
+        <v>930</v>
+      </c>
+      <c r="C17" s="6">
+        <v>41450</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1300</v>
+      </c>
+      <c r="E17" s="5">
+        <v>-2</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.9607843137254902E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>41496</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B18" s="12">
         <v>545</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C18" s="11">
         <v>41502</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D18" s="12">
         <v>1945</v>
       </c>
-      <c r="E16" s="15">
-        <f>F16*0.102*100</f>
+      <c r="E18" s="15">
+        <f>F18*0.102*100</f>
         <v>2.04</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F18" s="13">
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>41502</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B19" s="8">
         <v>2000</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C19" s="7">
         <v>41543</v>
       </c>
-      <c r="D17" s="8">
-        <v>1200</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="D19" s="8">
+        <v>1200</v>
+      </c>
+      <c r="E19" s="14">
         <v>4</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F19" s="9">
         <f t="shared" si="1"/>
         <v>3.9215686274509803E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>41680</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C20" s="6">
         <v>41684</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D20" s="1">
         <v>1615</v>
       </c>
-      <c r="E18" s="3">
-        <f t="shared" ref="E18:E22" si="2">F18*0.102*100</f>
+      <c r="E20" s="3">
+        <f t="shared" ref="E20:E24" si="2">F20*0.102*100</f>
         <v>3.6719999999999997</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F20" s="4">
         <v>0.36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>41684</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B21" s="1">
         <v>1630</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C21" s="6">
         <v>41849</v>
       </c>
-      <c r="D19" s="1">
-        <v>1200</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D21" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="3">
         <f t="shared" si="2"/>
         <v>3.0599999999999996</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F21" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>41849</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B22" s="1">
         <v>1215</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C22" s="6">
         <v>41907</v>
       </c>
-      <c r="D20" s="1">
-        <v>1200</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D22" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E22" s="3">
         <f t="shared" si="2"/>
         <v>6.4260000000000002</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F22" s="4">
         <v>0.63</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>41913</v>
       </c>
-      <c r="B21" s="1">
-        <v>1200</v>
-      </c>
-      <c r="C21" s="6">
+      <c r="B23" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C23" s="6">
         <v>41977</v>
       </c>
-      <c r="D21" s="1">
-        <v>1200</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D23" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E23" s="3">
         <f t="shared" si="2"/>
         <v>4.3859999999999992</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F23" s="4">
         <v>0.43</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>41977</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B24" s="1">
         <v>1215</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C24" s="6">
         <v>41992</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D24" s="1">
         <v>230</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E24" s="3">
         <f t="shared" si="2"/>
         <v>3.0599999999999996</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F24" s="4">
         <v>0.3</v>
       </c>
     </row>
@@ -892,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>